<commit_message>
5 literatur review CS
</commit_message>
<xml_diff>
--- a/Tugas Cyber Security/Cyber Security.xlsx
+++ b/Tugas Cyber Security/Cyber Security.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\filbe\OneDrive\Dokumen\Metodologi Penelitian\Tugas Cyber Security\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5FA60C0-0F39-4BA3-AD44-7797D6B68FB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F7D5286-13B5-4776-AE80-860F9C506B88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-118" yWindow="-118" windowWidth="25370" windowHeight="15225" xr2:uid="{1A90EFCB-5F87-43B7-ABE3-D8B5D4814BDE}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="73">
   <si>
     <t xml:space="preserve">Judul </t>
   </si>
@@ -97,9 +97,6 @@
   </si>
   <si>
     <t>Studi ini membahas peningkatan ancaman siber akibat digitalisasi, terutama pada keamanan cloud. Penelitian ini bertujuan untuk mengeksplorasi metodologi dan teknologi mutakhir untuk mendeteksi dan mengurangi serangan siber yang semakin kompleks.</t>
-  </si>
-  <si>
-    <t>12-Maret-2024</t>
   </si>
   <si>
     <t>Jurnal ini mengimplementasikan metodologi analisis konseptual yang mengidentifikasi kerentanan keamanan, metodologi deteksi, serta strategi mitigasi menggunakan teknologi terkini.</t>
@@ -122,10 +119,145 @@
 Solusi non-teknis dibahas, namun kelayakan implementasi di aplikasi nyata kurang mendalam.</t>
   </si>
   <si>
-    <t xml:space="preserve"> 5/5</t>
-  </si>
-  <si>
     <t>10/26/2024 Filbert Wijaya</t>
+  </si>
+  <si>
+    <t>Security Attacks in Cloud Computing and Corresponding Defending Mechanisms</t>
+  </si>
+  <si>
+    <t>Hesham Abusaimeh</t>
+  </si>
+  <si>
+    <t>Maret-2024</t>
+  </si>
+  <si>
+    <t>Mei-Juni 2020</t>
+  </si>
+  <si>
+    <t>International Journal of Advanced Trends in Computer Science and Engineering</t>
+  </si>
+  <si>
+    <t>Jurnal mengkaji berbagai serangan keamanan pada cloud computing, termasuk serangan brute force, replay, phishing, man-in-the-middle, dan lainnya.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Menggunakan pendekatan survei untuk meninjau serangan autentikasi di cloud dan studi-studi terkait pertahanan.</t>
+  </si>
+  <si>
+    <t>Menggunakan literatur untuk mengidentifikasi serangan dan solusi pertahanan terkait.</t>
+  </si>
+  <si>
+    <t>K-means untuk deteksi brute force dan WS-Security untuk serangan MITM.</t>
+  </si>
+  <si>
+    <t>Kombinasi berbagai mekanisme protektif, seperti password berbasis gambar, dapat mengurangi risiko serangan autentikasi.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Memberikan ulasan komprehensif tentang jenis serangan keamanan di cloud dan solusi untuk setiap jenis serangan.</t>
+  </si>
+  <si>
+    <t>Tidak mencakup solusi mendalam untuk semua jenis serangan dan tidak menguji efektivitas solusi.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10/27/2024 Filbert Wijaya </t>
+  </si>
+  <si>
+    <t>Cloud Security Issues in Present Day Context</t>
+  </si>
+  <si>
+    <t>Zhimin Guan, Dr. Rama Bhatia</t>
+  </si>
+  <si>
+    <t>Desember 2022</t>
+  </si>
+  <si>
+    <t>ScienceOpen Preprints</t>
+  </si>
+  <si>
+    <t>Isu utama keamanan cloud, multi-tenancy, dan risiko model layanan cloud seperti IaaS, PaaS, SaaS</t>
+  </si>
+  <si>
+    <t>Studi kualitatif berbasis literatur yang menggunakan pendekatan sistematis (PRISMA) untuk memilih artikel terkait cloud security dari sumber tepercaya seperti IEEE dan Springer.</t>
+  </si>
+  <si>
+    <t>Analisis teks untuk menyusun dan mengelompokkan ancaman keamanan cloud, tanpa penggunaan uji praktis atau alat AI.</t>
+  </si>
+  <si>
+    <t>Klasifikasi ancaman keamanan berdasarkan level layanan dan model penyebaran cloud.</t>
+  </si>
+  <si>
+    <t>Daftar ancaman cloud, teknik mitigasi seperti enkripsi dan pengelolaan kunci.</t>
+  </si>
+  <si>
+    <t>Komprehensif dan terstruktur dalam klasifikasi ancaman keamanan.</t>
+  </si>
+  <si>
+    <t>Tidak ada uji praktis atau contoh implementasi mitigasi.</t>
+  </si>
+  <si>
+    <t>Securing Machine Learning in the Cloud: A Systematic Review of Cloud Machine Learning Security</t>
+  </si>
+  <si>
+    <t>Adnan Qayyum, Aneeqa Ijaz, Muhammad Usama, Waleed Iqbal, Junaid Qadir, Yehia Elkhatib, Ala Al-Fuqaha</t>
+  </si>
+  <si>
+    <t>Novemberr 2020</t>
+  </si>
+  <si>
+    <t>Frontiers in Big Data</t>
+  </si>
+  <si>
+    <t>Keamanan Machine Learning as a Service (MLaaS) dan tantangan serangan serta pertahanan pada cloud ML/DL.</t>
+  </si>
+  <si>
+    <t>Tinjauan sistematis menggunakan protokol PRISMA untuk memilih artikel terkait dari delapan pustaka utama.</t>
+  </si>
+  <si>
+    <t>Analisis literatur pada serangan dan metode pertahanan untuk cloud-hosted ML/DL, dengan fokus pada serangan dan mitigasinya.</t>
+  </si>
+  <si>
+    <t>Tidak ada algoritma spesifik yang dikembangkan; penelitian mengkategorikan tipe serangan dan pertahanan terhadap cloud-hosted ML/DL.</t>
+  </si>
+  <si>
+    <t>Mengidentifikasi ancaman seperti serangan black-box, white-box, dan metode mitigasi seperti homomorphic encryption.</t>
+  </si>
+  <si>
+    <t>Artikel ini menyajikan ikhtisar komprehensif mengenai serangan dan pertahanan pada cloud ML/DL, serta menyusun taksonomi yang terperinci.</t>
+  </si>
+  <si>
+    <t>Tidak ada eksperimen langsung untuk mengevaluasi efektivitas pertahanan yang diusulkan.</t>
+  </si>
+  <si>
+    <t>Effective Intrusion Detection System to Secure Data in Cloud Using Machine Learning</t>
+  </si>
+  <si>
+    <t>Ammar Aldallal, Faisal Alisa</t>
+  </si>
+  <si>
+    <t>Desember 2021</t>
+  </si>
+  <si>
+    <t>MDPI Symmetry</t>
+  </si>
+  <si>
+    <t>Mendeteksi dan melindungi data cloud dari serangan intrusi dengan sistem deteksi intrusi berbasis machine learning.</t>
+  </si>
+  <si>
+    <t>Studi berbasis eksperimen menggunakan dataset CICIDS2017 untuk menguji sistem deteksi intrusi yang diusulkan.</t>
+  </si>
+  <si>
+    <t>Menggabungkan algoritma Support Vector Machine (SVM) dan Genetic Algorithm (GA) untuk meningkatkan akurasi sistem.</t>
+  </si>
+  <si>
+    <t>Support Vector Machine (SVM) dan Genetic Algorithm (GA) digunakan secara paralel untuk memilih fitur dan meningkatkan akurasi.</t>
+  </si>
+  <si>
+    <t>Model ini menunjukkan peningkatan performa hingga 5.74% dibandingkan benchmark lain menggunakan dataset KDD CUP 99 dan NSL-KDD.</t>
+  </si>
+  <si>
+    <t>Efisiensi tinggi dalam mendeteksi serangan cloud melalui kombinasi GA dan SVM, meningkatkan simetri antara keamanan data dan deteksi intrusi.</t>
+  </si>
+  <si>
+    <t>Hanya diuji menggunakan dataset CICIDS2017, tidak mencakup uji dunia nyata atau implementasi langsung di cloud.</t>
   </si>
 </sst>
 </file>
@@ -155,7 +287,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -193,17 +325,6 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -215,25 +336,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -244,12 +375,54 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -564,19 +737,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{129348A8-1C1A-4064-979B-57C2723345AF}">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J92"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="D55" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D92" sqref="D92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="59.5546875" customWidth="1"/>
-    <col min="4" max="4" width="46.33203125" customWidth="1"/>
-    <col min="5" max="5" width="13.77734375" customWidth="1"/>
-    <col min="6" max="6" width="43.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="94.88671875" customWidth="1"/>
+    <col min="4" max="4" width="51.33203125" customWidth="1"/>
+    <col min="5" max="5" width="16.77734375" customWidth="1"/>
+    <col min="6" max="6" width="76.77734375" customWidth="1"/>
     <col min="7" max="7" width="55.77734375" customWidth="1"/>
     <col min="8" max="9" width="39.44140625" customWidth="1"/>
     <col min="10" max="10" width="68.5546875" customWidth="1"/>
@@ -602,7 +775,7 @@
         <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -621,111 +794,661 @@
       <c r="F5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="1" t="s">
+    </row>
+    <row r="6" spans="1:10" ht="22.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="25.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="D8" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="E8" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="F8" s="14"/>
+      <c r="G8" s="12" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="140.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="9" t="s">
+      <c r="H8" s="12"/>
+    </row>
+    <row r="9" spans="1:10" ht="122.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="H6" s="10" t="s">
+      <c r="E9" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="I6" s="10" t="s">
+      <c r="F9" s="19"/>
+      <c r="G9" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="J6" s="11" t="s">
+      <c r="H9" s="17"/>
+    </row>
+    <row r="11" spans="1:10" ht="19.649999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="14"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+    </row>
+    <row r="12" spans="1:10" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="16"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="75.3" x14ac:dyDescent="0.3">
+      <c r="C15" s="5" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C7" s="2" t="s">
+      <c r="D15" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C19" s="23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C21" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C23" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F23" s="14"/>
+      <c r="G23" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H23" s="14"/>
+    </row>
+    <row r="24" spans="2:8" ht="45.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C24" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E24" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="F24" s="22"/>
+      <c r="G24" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="H24" s="22"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C26" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="4"/>
-    </row>
-    <row r="8" spans="1:10" ht="25.55" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="7"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C10" s="1" t="s">
+      <c r="D26" s="14"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+    </row>
+    <row r="27" spans="2:8" ht="15.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C27" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D27" s="7"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C29" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D29" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="61.55" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C13" s="1" t="s">
+    <row r="30" spans="2:8" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="C30" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C32" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="13" t="s">
-        <v>27</v>
+      <c r="D32" s="20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B35">
+        <v>3</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="2"/>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C38" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D38" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E38" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F38" s="14"/>
+      <c r="G38" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H38" s="14"/>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="21"/>
+      <c r="F39" s="22"/>
+      <c r="G39" s="21"/>
+      <c r="H39" s="22"/>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C41" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D41" s="14"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="10"/>
+      <c r="H41" s="10"/>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C42" s="6"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
+      <c r="G42" s="9"/>
+      <c r="H42" s="9"/>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C44" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C47" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D47" s="20"/>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B50">
+        <v>4</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C51" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C53" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D53" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E53" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F53" s="14"/>
+      <c r="G53" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H53" s="14"/>
+    </row>
+    <row r="54" spans="2:8" ht="60.25" x14ac:dyDescent="0.3">
+      <c r="C54" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E54" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="F54" s="22"/>
+      <c r="G54" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="H54" s="22"/>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C56" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D56" s="14"/>
+      <c r="E56" s="10"/>
+      <c r="F56" s="10"/>
+      <c r="G56" s="10"/>
+      <c r="H56" s="10"/>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C57" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D57" s="7"/>
+      <c r="E57" s="9"/>
+      <c r="F57" s="9"/>
+      <c r="G57" s="9"/>
+      <c r="H57" s="9"/>
+    </row>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C59" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="60" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C60" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="62" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C62" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D62" s="20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="65" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B65">
+        <v>5</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="2:8" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="C66" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D66" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C68" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D68" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E68" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F68" s="14"/>
+      <c r="G68" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H68" s="14"/>
+    </row>
+    <row r="69" spans="2:8" ht="45.2" x14ac:dyDescent="0.3">
+      <c r="C69" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E69" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="F69" s="22"/>
+      <c r="G69" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="H69" s="22"/>
+    </row>
+    <row r="71" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C71" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D71" s="14"/>
+      <c r="E71" s="10"/>
+      <c r="F71" s="10"/>
+      <c r="G71" s="10"/>
+      <c r="H71" s="10"/>
+    </row>
+    <row r="72" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C72" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D72" s="7"/>
+      <c r="E72" s="9"/>
+      <c r="F72" s="9"/>
+      <c r="G72" s="9"/>
+      <c r="H72" s="9"/>
+    </row>
+    <row r="74" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C74" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="75" spans="2:8" ht="47.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C75" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D75" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="77" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C77" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D77" s="20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="80" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B80">
+        <v>6</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="81" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C81" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D81" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E81" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="83" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C83" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D83" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E83" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F83" s="14"/>
+      <c r="G83" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H83" s="14"/>
+    </row>
+    <row r="84" spans="3:8" ht="47.15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C84" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D84" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E84" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="F84" s="22"/>
+      <c r="G84" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="H84" s="22"/>
+    </row>
+    <row r="86" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C86" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D86" s="14"/>
+      <c r="E86" s="10"/>
+      <c r="F86" s="10"/>
+      <c r="G86" s="10"/>
+      <c r="H86" s="10"/>
+    </row>
+    <row r="87" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C87" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D87" s="7"/>
+      <c r="E87" s="9"/>
+      <c r="F87" s="9"/>
+      <c r="G87" s="9"/>
+      <c r="H87" s="9"/>
+    </row>
+    <row r="89" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C89" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="90" spans="3:8" ht="44.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C90" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="D90" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="92" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C92" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D92" s="20">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="C8:J8"/>
+  <mergeCells count="36">
+    <mergeCell ref="C86:D86"/>
+    <mergeCell ref="C87:D87"/>
+    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="C72:D72"/>
+    <mergeCell ref="E83:F83"/>
+    <mergeCell ref="G83:H83"/>
+    <mergeCell ref="E84:F84"/>
+    <mergeCell ref="G84:H84"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="E68:F68"/>
+    <mergeCell ref="G68:H68"/>
+    <mergeCell ref="E69:F69"/>
+    <mergeCell ref="G69:H69"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E53:F53"/>
+    <mergeCell ref="G53:H53"/>
+    <mergeCell ref="E54:F54"/>
+    <mergeCell ref="G54:H54"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="C11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003C7AD250DB415C4FB5867649A57761AA" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5453886a6cd3b6f266e49a5bb2bbff1b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="89c1253a-f7ad-4028-b395-8ef7f6c6d0dc" xmlns:ns4="84555582-1fd8-462d-916c-584d43361c96" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2ff136199dbbf9c5158804c9410598b8" ns3:_="" ns4:_="">
     <xsd:import namespace="89c1253a-f7ad-4028-b395-8ef7f6c6d0dc"/>
@@ -964,6 +1687,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -973,14 +1705,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5FBC2FF6-442F-42BA-AF7E-A1EAD5DFC796}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29BFF3F2-E4BC-493A-A0DA-3AF5FC7C25C2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -995,6 +1719,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5FBC2FF6-442F-42BA-AF7E-A1EAD5DFC796}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>